<commit_message>
added listener and calculations for ecu can stream.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3381" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6322" uniqueCount="165">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -465,6 +465,51 @@
   </si>
   <si>
     <t xml:space="preserve">KMH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rpm_letters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; RPM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rpm_descriptor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EGT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">740</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OIL. T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OIL. P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oil. P</t>
   </si>
 </sst>
 </file>
@@ -1704,10 +1749,10 @@
         <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D4">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -1922,6 +1967,29 @@
       </c>
     </row>
     <row r="10" spans="2:16">
+      <c r="B10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10">
+        <v>21</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10"/>
+      <c r="I10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10"/>
       <c r="L10" s="11" t="s">
         <v>36</v>
       </c>
@@ -1937,6 +2005,25 @@
       <c r="P10" s="14"/>
     </row>
     <row r="11" spans="2:16">
+      <c r="B11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
       <c r="L11" s="15"/>
     </row>
     <row r="12" spans="2:16">
@@ -2438,7 +2525,7 @@
         <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>74</v>
+        <v>161</v>
       </c>
       <c r="F28" t="s">
         <v>58</v>
@@ -2472,7 +2559,7 @@
         <v>80</v>
       </c>
       <c r="E30" t="s">
-        <v>124</v>
+        <v>160</v>
       </c>
       <c r="F30" t="s">
         <v>58</v>
@@ -2523,7 +2610,7 @@
         <v>80</v>
       </c>
       <c r="E33" t="s">
-        <v>131</v>
+        <v>162</v>
       </c>
       <c r="F33" t="s">
         <v>58</v>
@@ -2540,7 +2627,7 @@
         <v>80</v>
       </c>
       <c r="E34" t="s">
-        <v>133</v>
+        <v>163</v>
       </c>
       <c r="F34" t="s">
         <v>58</v>
@@ -2670,7 +2757,7 @@
         <v>145</v>
       </c>
       <c r="C42" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="D42" t="s">
         <v>80</v>
@@ -2687,7 +2774,7 @@
         <v>147</v>
       </c>
       <c r="C43" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="D43" t="s">
         <v>80</v>
@@ -2699,9 +2786,57 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
+    <row r="44">
+      <c r="B44" t="s">
+        <v>151</v>
+      </c>
+      <c r="C44" t="s">
+        <v>150</v>
+      </c>
+      <c r="D44" t="s">
+        <v>152</v>
+      </c>
+      <c r="E44" t="s">
+        <v>156</v>
+      </c>
+      <c r="F44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="s">
+        <v>154</v>
+      </c>
+      <c r="C45" t="s">
+        <v>150</v>
+      </c>
+      <c r="D45" t="s">
+        <v>80</v>
+      </c>
+      <c r="E45" t="s">
+        <v>157</v>
+      </c>
+      <c r="F45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="s">
+        <v>158</v>
+      </c>
+      <c r="C46" t="s">
+        <v>155</v>
+      </c>
+      <c r="D46" t="s">
+        <v>80</v>
+      </c>
+      <c r="E46" t="s">
+        <v>159</v>
+      </c>
+      <c r="F46" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="47"/>
     <row r="48"/>
     <row r="49"/>

</xml_diff>

<commit_message>
updated with batt, tps, egt, iat, etc.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6322" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7490" uniqueCount="172">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -510,6 +510,27 @@
   </si>
   <si>
     <t xml:space="preserve">Oil. P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId56</t>
   </si>
 </sst>
 </file>
@@ -2108,10 +2129,10 @@
     </row>
     <row r="4" spans="2:10" ht="15" customHeight="1">
       <c r="B4" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="D4" t="s">
         <v>57</v>
@@ -2125,16 +2146,16 @@
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1">
       <c r="B5" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="D5" t="s">
         <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>114</v>
+        <v>74</v>
       </c>
       <c r="F5" t="s">
         <v>58</v>
@@ -2142,7 +2163,7 @@
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
         <v>51</v>
@@ -2159,7 +2180,7 @@
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C7" t="s">
         <v>51</v>
@@ -2168,7 +2189,7 @@
         <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F7" t="s">
         <v>58</v>
@@ -2176,16 +2197,16 @@
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="D8" t="s">
         <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="F8" t="s">
         <v>58</v>
@@ -2193,16 +2214,16 @@
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="F9" t="s">
         <v>58</v>
@@ -2210,16 +2231,16 @@
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D10" t="s">
         <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="F10" t="s">
         <v>58</v>
@@ -2227,16 +2248,16 @@
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D11" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="F11" t="s">
         <v>58</v>
@@ -2244,16 +2265,16 @@
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="D12" t="s">
         <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="F12" t="s">
         <v>58</v>
@@ -2261,16 +2282,16 @@
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="D13" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="F13" t="s">
         <v>58</v>
@@ -2278,7 +2299,7 @@
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="C14" t="s">
         <v>92</v>
@@ -2287,7 +2308,7 @@
         <v>57</v>
       </c>
       <c r="E14" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="F14" t="s">
         <v>58</v>
@@ -2295,7 +2316,7 @@
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="C15" t="s">
         <v>92</v>
@@ -2304,7 +2325,7 @@
         <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="F15" t="s">
         <v>58</v>
@@ -2312,7 +2333,7 @@
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C16" t="s">
         <v>92</v>
@@ -2321,7 +2342,7 @@
         <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="F16" t="s">
         <v>58</v>
@@ -2329,7 +2350,7 @@
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="C17" t="s">
         <v>92</v>
@@ -2338,7 +2359,7 @@
         <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="F17" t="s">
         <v>58</v>
@@ -2346,16 +2367,16 @@
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="C18" t="s">
         <v>92</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E18" t="s">
-        <v>102</v>
+        <v>149</v>
       </c>
       <c r="F18" t="s">
         <v>58</v>
@@ -2363,16 +2384,16 @@
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="D19" t="s">
         <v>57</v>
       </c>
       <c r="E19" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="F19" t="s">
         <v>58</v>
@@ -2380,16 +2401,16 @@
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="C20" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E20" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="F20" t="s">
         <v>58</v>
@@ -2397,16 +2418,16 @@
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D21" t="s">
         <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="F21" t="s">
         <v>58</v>
@@ -2414,16 +2435,16 @@
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D22" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E22" t="s">
-        <v>110</v>
+        <v>161</v>
       </c>
       <c r="F22" t="s">
         <v>58</v>
@@ -2431,16 +2452,16 @@
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="C23" t="s">
         <v>92</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E23" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="F23" t="s">
         <v>58</v>
@@ -2448,7 +2469,7 @@
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="C24" t="s">
         <v>92</v>
@@ -2457,7 +2478,7 @@
         <v>80</v>
       </c>
       <c r="E24" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="F24" t="s">
         <v>58</v>
@@ -2465,16 +2486,16 @@
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E25" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
       <c r="F25" t="s">
         <v>58</v>
@@ -2482,16 +2503,16 @@
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="D26" t="s">
         <v>80</v>
       </c>
       <c r="E26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F26" t="s">
         <v>58</v>
@@ -2499,16 +2520,16 @@
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D27" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E27" t="s">
-        <v>81</v>
+        <v>162</v>
       </c>
       <c r="F27" t="s">
         <v>58</v>
@@ -2516,16 +2537,16 @@
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D28" t="s">
         <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F28" t="s">
         <v>58</v>
@@ -2533,16 +2554,16 @@
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="D29" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E29" t="s">
-        <v>122</v>
+        <v>81</v>
       </c>
       <c r="F29" t="s">
         <v>58</v>
@@ -2550,16 +2571,16 @@
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="D30" t="s">
         <v>80</v>
       </c>
       <c r="E30" t="s">
-        <v>160</v>
+        <v>78</v>
       </c>
       <c r="F30" t="s">
         <v>58</v>
@@ -2567,16 +2588,16 @@
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E31" t="s">
-        <v>126</v>
+        <v>81</v>
       </c>
       <c r="F31" t="s">
         <v>58</v>
@@ -2584,16 +2605,16 @@
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D32" t="s">
         <v>80</v>
       </c>
       <c r="E32" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="F32" t="s">
         <v>58</v>
@@ -2601,7 +2622,7 @@
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="C33" t="s">
         <v>92</v>
@@ -2610,7 +2631,7 @@
         <v>80</v>
       </c>
       <c r="E33" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="F33" t="s">
         <v>58</v>
@@ -2618,7 +2639,7 @@
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="C34" t="s">
         <v>92</v>
@@ -2627,7 +2648,7 @@
         <v>80</v>
       </c>
       <c r="E34" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="F34" t="s">
         <v>58</v>
@@ -2635,16 +2656,16 @@
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C35" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="D35" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E35" t="s">
-        <v>81</v>
+        <v>144</v>
       </c>
       <c r="F35" t="s">
         <v>58</v>
@@ -2652,16 +2673,16 @@
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="C36" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D36" t="s">
         <v>80</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
+        <v>146</v>
       </c>
       <c r="F36" t="s">
         <v>58</v>
@@ -2669,16 +2690,16 @@
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="C37" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E37" t="s">
-        <v>81</v>
+        <v>148</v>
       </c>
       <c r="F37" t="s">
         <v>58</v>
@@ -2686,16 +2707,16 @@
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="C38" t="s">
-        <v>91</v>
+        <v>150</v>
       </c>
       <c r="D38" t="s">
-        <v>80</v>
+        <v>152</v>
       </c>
       <c r="E38" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="F38" t="s">
         <v>58</v>
@@ -2703,16 +2724,16 @@
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="C39" t="s">
-        <v>92</v>
+        <v>150</v>
       </c>
       <c r="D39" t="s">
         <v>80</v>
       </c>
       <c r="E39" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="F39" t="s">
         <v>58</v>
@@ -2720,16 +2741,16 @@
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="C40" t="s">
-        <v>92</v>
+        <v>155</v>
       </c>
       <c r="D40" t="s">
         <v>80</v>
       </c>
       <c r="E40" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="F40" t="s">
         <v>58</v>
@@ -2737,16 +2758,16 @@
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="C41" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="D41" t="s">
-        <v>80</v>
+        <v>152</v>
       </c>
       <c r="E41" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="F41" t="s">
         <v>58</v>
@@ -2754,16 +2775,16 @@
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="C42" t="s">
-        <v>40</v>
+        <v>113</v>
       </c>
       <c r="D42" t="s">
         <v>80</v>
       </c>
       <c r="E42" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="F42" t="s">
         <v>58</v>
@@ -2771,16 +2792,16 @@
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D43" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E43" t="s">
-        <v>148</v>
+        <v>81</v>
       </c>
       <c r="F43" t="s">
         <v>58</v>
@@ -2788,16 +2809,16 @@
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>151</v>
+        <v>168</v>
       </c>
       <c r="C44" t="s">
-        <v>150</v>
+        <v>51</v>
       </c>
       <c r="D44" t="s">
-        <v>152</v>
+        <v>80</v>
       </c>
       <c r="E44" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="F44" t="s">
         <v>58</v>
@@ -2805,16 +2826,16 @@
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="C45" t="s">
-        <v>150</v>
+        <v>51</v>
       </c>
       <c r="D45" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E45" t="s">
-        <v>157</v>
+        <v>81</v>
       </c>
       <c r="F45" t="s">
         <v>58</v>
@@ -2822,16 +2843,16 @@
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="C46" t="s">
-        <v>155</v>
+        <v>51</v>
       </c>
       <c r="D46" t="s">
         <v>80</v>
       </c>
       <c r="E46" t="s">
-        <v>159</v>
+        <v>72</v>
       </c>
       <c r="F46" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
added rpm flashing light
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7490" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8965" uniqueCount="178">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -531,6 +531,24 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10000</t>
   </si>
 </sst>
 </file>
@@ -2605,16 +2623,16 @@
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D32" t="s">
         <v>80</v>
       </c>
       <c r="E32" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F32" t="s">
         <v>58</v>
@@ -2622,7 +2640,7 @@
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C33" t="s">
         <v>92</v>
@@ -2631,7 +2649,7 @@
         <v>80</v>
       </c>
       <c r="E33" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F33" t="s">
         <v>58</v>
@@ -2639,7 +2657,7 @@
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C34" t="s">
         <v>92</v>
@@ -2648,7 +2666,7 @@
         <v>80</v>
       </c>
       <c r="E34" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F34" t="s">
         <v>58</v>
@@ -2656,16 +2674,16 @@
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C35" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="D35" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E35" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F35" t="s">
         <v>58</v>
@@ -2673,7 +2691,7 @@
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C36" t="s">
         <v>40</v>
@@ -2682,7 +2700,7 @@
         <v>80</v>
       </c>
       <c r="E36" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F36" t="s">
         <v>58</v>
@@ -2690,16 +2708,16 @@
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C37" t="s">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="D37" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E37" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="F37" t="s">
         <v>58</v>
@@ -2707,16 +2725,16 @@
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C38" t="s">
         <v>150</v>
       </c>
       <c r="D38" t="s">
-        <v>152</v>
+        <v>80</v>
       </c>
       <c r="E38" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="F38" t="s">
         <v>58</v>
@@ -2724,16 +2742,16 @@
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C39" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="D39" t="s">
         <v>80</v>
       </c>
       <c r="E39" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F39" t="s">
         <v>58</v>
@@ -2741,16 +2759,16 @@
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="C40" t="s">
-        <v>155</v>
+        <v>51</v>
       </c>
       <c r="D40" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E40" t="s">
-        <v>159</v>
+        <v>81</v>
       </c>
       <c r="F40" t="s">
         <v>58</v>
@@ -2758,16 +2776,16 @@
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C41" t="s">
-        <v>113</v>
+        <v>51</v>
       </c>
       <c r="D41" t="s">
-        <v>152</v>
+        <v>80</v>
       </c>
       <c r="E41" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="F41" t="s">
         <v>58</v>
@@ -2775,16 +2793,16 @@
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C42" t="s">
-        <v>113</v>
+        <v>51</v>
       </c>
       <c r="D42" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E42" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="F42" t="s">
         <v>58</v>
@@ -2792,16 +2810,16 @@
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C43" t="s">
         <v>51</v>
       </c>
       <c r="D43" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E43" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="F43" t="s">
         <v>58</v>
@@ -2809,16 +2827,16 @@
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="D44" t="s">
         <v>80</v>
       </c>
       <c r="E44" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="F44" t="s">
         <v>58</v>
@@ -2826,10 +2844,10 @@
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C45" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="D45" t="s">
         <v>57</v>
@@ -2843,16 +2861,16 @@
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C46" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="D46" t="s">
         <v>80</v>
       </c>
       <c r="E46" t="s">
-        <v>72</v>
+        <v>176</v>
       </c>
       <c r="F46" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
added customization to the rev bar graphics
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8965" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9639" uniqueCount="188">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -549,6 +549,36 @@
   </si>
   <si>
     <t xml:space="preserve">10000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId69</t>
   </si>
 </sst>
 </file>
@@ -2224,7 +2254,7 @@
         <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="F8" t="s">
         <v>58</v>
@@ -2241,7 +2271,7 @@
         <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="F9" t="s">
         <v>58</v>
@@ -2258,7 +2288,7 @@
         <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="F10" t="s">
         <v>58</v>
@@ -2275,7 +2305,7 @@
         <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="F11" t="s">
         <v>58</v>
@@ -2292,7 +2322,7 @@
         <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="F12" t="s">
         <v>58</v>
@@ -2309,7 +2339,7 @@
         <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="F13" t="s">
         <v>58</v>
@@ -2326,7 +2356,7 @@
         <v>57</v>
       </c>
       <c r="E14" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="F14" t="s">
         <v>58</v>
@@ -2343,7 +2373,7 @@
         <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="F15" t="s">
         <v>58</v>
@@ -2360,7 +2390,7 @@
         <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="F16" t="s">
         <v>58</v>
@@ -2377,7 +2407,7 @@
         <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="F17" t="s">
         <v>58</v>
@@ -2876,12 +2906,176 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
+    <row r="47">
+      <c r="B47" t="s">
+        <v>178</v>
+      </c>
+      <c r="C47" t="s">
+        <v>92</v>
+      </c>
+      <c r="D47" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" t="s">
+        <v>94</v>
+      </c>
+      <c r="F47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="s">
+        <v>179</v>
+      </c>
+      <c r="C48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" t="s">
+        <v>80</v>
+      </c>
+      <c r="E48" t="s">
+        <v>96</v>
+      </c>
+      <c r="F48" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="s">
+        <v>180</v>
+      </c>
+      <c r="C49" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" t="s">
+        <v>80</v>
+      </c>
+      <c r="E49" t="s">
+        <v>98</v>
+      </c>
+      <c r="F49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="s">
+        <v>181</v>
+      </c>
+      <c r="C50" t="s">
+        <v>92</v>
+      </c>
+      <c r="D50" t="s">
+        <v>80</v>
+      </c>
+      <c r="E50" t="s">
+        <v>100</v>
+      </c>
+      <c r="F50" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="s">
+        <v>182</v>
+      </c>
+      <c r="C51" t="s">
+        <v>92</v>
+      </c>
+      <c r="D51" t="s">
+        <v>80</v>
+      </c>
+      <c r="E51" t="s">
+        <v>102</v>
+      </c>
+      <c r="F51" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="s">
+        <v>183</v>
+      </c>
+      <c r="C52" t="s">
+        <v>92</v>
+      </c>
+      <c r="D52" t="s">
+        <v>80</v>
+      </c>
+      <c r="E52" t="s">
+        <v>104</v>
+      </c>
+      <c r="F52" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="s">
+        <v>184</v>
+      </c>
+      <c r="C53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D53" t="s">
+        <v>80</v>
+      </c>
+      <c r="E53" t="s">
+        <v>106</v>
+      </c>
+      <c r="F53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" t="s">
+        <v>185</v>
+      </c>
+      <c r="C54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D54" t="s">
+        <v>80</v>
+      </c>
+      <c r="E54" t="s">
+        <v>108</v>
+      </c>
+      <c r="F54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" t="s">
+        <v>186</v>
+      </c>
+      <c r="C55" t="s">
+        <v>92</v>
+      </c>
+      <c r="D55" t="s">
+        <v>80</v>
+      </c>
+      <c r="E55" t="s">
+        <v>110</v>
+      </c>
+      <c r="F55" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" t="s">
+        <v>187</v>
+      </c>
+      <c r="C56" t="s">
+        <v>92</v>
+      </c>
+      <c r="D56" t="s">
+        <v>80</v>
+      </c>
+      <c r="E56" t="s">
+        <v>112</v>
+      </c>
+      <c r="F56" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="0" objects="0" scenarios="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
change to 8000rpm max value
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9639" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9970" uniqueCount="189">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -579,6 +579,9 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7200</t>
   </si>
 </sst>
 </file>
@@ -2381,16 +2384,16 @@
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C16" t="s">
         <v>92</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E16" t="s">
-        <v>81</v>
+        <v>149</v>
       </c>
       <c r="F16" t="s">
         <v>58</v>
@@ -2398,10 +2401,10 @@
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
         <v>57</v>
@@ -2415,16 +2418,16 @@
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C18" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="D18" t="s">
         <v>80</v>
       </c>
       <c r="E18" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="F18" t="s">
         <v>58</v>
@@ -2432,10 +2435,10 @@
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="D19" t="s">
         <v>57</v>
@@ -2449,16 +2452,16 @@
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="D20" t="s">
         <v>80</v>
       </c>
       <c r="E20" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="F20" t="s">
         <v>58</v>
@@ -2466,16 +2469,16 @@
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E21" t="s">
-        <v>81</v>
+        <v>122</v>
       </c>
       <c r="F21" t="s">
         <v>58</v>
@@ -2483,16 +2486,16 @@
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D22" t="s">
         <v>80</v>
       </c>
       <c r="E22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F22" t="s">
         <v>58</v>
@@ -2500,7 +2503,7 @@
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C23" t="s">
         <v>92</v>
@@ -2509,7 +2512,7 @@
         <v>80</v>
       </c>
       <c r="E23" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F23" t="s">
         <v>58</v>
@@ -2517,7 +2520,7 @@
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C24" t="s">
         <v>92</v>
@@ -2526,7 +2529,7 @@
         <v>80</v>
       </c>
       <c r="E24" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="F24" t="s">
         <v>58</v>
@@ -2534,7 +2537,7 @@
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C25" t="s">
         <v>92</v>
@@ -2543,7 +2546,7 @@
         <v>80</v>
       </c>
       <c r="E25" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="F25" t="s">
         <v>58</v>
@@ -2551,7 +2554,7 @@
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C26" t="s">
         <v>92</v>
@@ -2560,7 +2563,7 @@
         <v>80</v>
       </c>
       <c r="E26" t="s">
-        <v>128</v>
+        <v>163</v>
       </c>
       <c r="F26" t="s">
         <v>58</v>
@@ -2568,16 +2571,16 @@
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="D27" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E27" t="s">
-        <v>162</v>
+        <v>81</v>
       </c>
       <c r="F27" t="s">
         <v>58</v>
@@ -2585,16 +2588,16 @@
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="D28" t="s">
         <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>163</v>
+        <v>78</v>
       </c>
       <c r="F28" t="s">
         <v>58</v>
@@ -2602,10 +2605,10 @@
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="D29" t="s">
         <v>57</v>
@@ -2619,16 +2622,16 @@
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C30" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="D30" t="s">
         <v>80</v>
       </c>
       <c r="E30" t="s">
-        <v>78</v>
+        <v>140</v>
       </c>
       <c r="F30" t="s">
         <v>58</v>
@@ -2636,16 +2639,16 @@
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D31" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E31" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
       <c r="F31" t="s">
         <v>58</v>
@@ -2653,7 +2656,7 @@
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C32" t="s">
         <v>92</v>
@@ -2662,7 +2665,7 @@
         <v>80</v>
       </c>
       <c r="E32" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="F32" t="s">
         <v>58</v>
@@ -2670,16 +2673,16 @@
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C33" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E33" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F33" t="s">
         <v>58</v>
@@ -2687,16 +2690,16 @@
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C34" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="D34" t="s">
         <v>80</v>
       </c>
       <c r="E34" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="F34" t="s">
         <v>58</v>
@@ -2704,16 +2707,16 @@
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="D35" t="s">
         <v>57</v>
       </c>
       <c r="E35" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="F35" t="s">
         <v>58</v>
@@ -2721,16 +2724,16 @@
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="D36" t="s">
         <v>80</v>
       </c>
       <c r="E36" t="s">
-        <v>148</v>
+        <v>188</v>
       </c>
       <c r="F36" t="s">
         <v>58</v>
@@ -2738,16 +2741,16 @@
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="C37" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E37" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F37" t="s">
         <v>58</v>
@@ -2755,16 +2758,16 @@
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="C38" t="s">
-        <v>150</v>
+        <v>51</v>
       </c>
       <c r="D38" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E38" t="s">
-        <v>177</v>
+        <v>81</v>
       </c>
       <c r="F38" t="s">
         <v>58</v>
@@ -2772,16 +2775,16 @@
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="C39" t="s">
-        <v>155</v>
+        <v>51</v>
       </c>
       <c r="D39" t="s">
         <v>80</v>
       </c>
       <c r="E39" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="F39" t="s">
         <v>58</v>
@@ -2789,7 +2792,7 @@
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C40" t="s">
         <v>51</v>
@@ -2806,7 +2809,7 @@
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C41" t="s">
         <v>51</v>
@@ -2815,7 +2818,7 @@
         <v>80</v>
       </c>
       <c r="E41" t="s">
-        <v>169</v>
+        <v>72</v>
       </c>
       <c r="F41" t="s">
         <v>58</v>
@@ -2823,16 +2826,16 @@
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C42" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="D42" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E42" t="s">
-        <v>81</v>
+        <v>173</v>
       </c>
       <c r="F42" t="s">
         <v>58</v>
@@ -2840,16 +2843,16 @@
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C43" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="D43" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E43" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="F43" t="s">
         <v>58</v>
@@ -2857,16 +2860,16 @@
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C44" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="D44" t="s">
         <v>80</v>
       </c>
       <c r="E44" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F44" t="s">
         <v>58</v>
@@ -2874,16 +2877,16 @@
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C45" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="D45" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E45" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="F45" t="s">
         <v>58</v>
@@ -2891,16 +2894,16 @@
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="C46" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="D46" t="s">
         <v>80</v>
       </c>
       <c r="E46" t="s">
-        <v>176</v>
+        <v>96</v>
       </c>
       <c r="F46" t="s">
         <v>58</v>
@@ -2908,7 +2911,7 @@
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C47" t="s">
         <v>92</v>
@@ -2917,7 +2920,7 @@
         <v>80</v>
       </c>
       <c r="E47" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F47" t="s">
         <v>58</v>
@@ -2925,7 +2928,7 @@
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C48" t="s">
         <v>92</v>
@@ -2934,7 +2937,7 @@
         <v>80</v>
       </c>
       <c r="E48" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F48" t="s">
         <v>58</v>
@@ -2942,7 +2945,7 @@
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C49" t="s">
         <v>92</v>
@@ -2951,7 +2954,7 @@
         <v>80</v>
       </c>
       <c r="E49" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F49" t="s">
         <v>58</v>
@@ -2959,7 +2962,7 @@
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C50" t="s">
         <v>92</v>
@@ -2968,7 +2971,7 @@
         <v>80</v>
       </c>
       <c r="E50" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F50" t="s">
         <v>58</v>
@@ -2976,7 +2979,7 @@
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C51" t="s">
         <v>92</v>
@@ -2985,7 +2988,7 @@
         <v>80</v>
       </c>
       <c r="E51" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F51" t="s">
         <v>58</v>
@@ -2993,7 +2996,7 @@
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C52" t="s">
         <v>92</v>
@@ -3002,80 +3005,16 @@
         <v>80</v>
       </c>
       <c r="E52" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F52" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="53">
-      <c r="B53" t="s">
-        <v>184</v>
-      </c>
-      <c r="C53" t="s">
-        <v>92</v>
-      </c>
-      <c r="D53" t="s">
-        <v>80</v>
-      </c>
-      <c r="E53" t="s">
-        <v>106</v>
-      </c>
-      <c r="F53" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="B54" t="s">
-        <v>185</v>
-      </c>
-      <c r="C54" t="s">
-        <v>92</v>
-      </c>
-      <c r="D54" t="s">
-        <v>80</v>
-      </c>
-      <c r="E54" t="s">
-        <v>108</v>
-      </c>
-      <c r="F54" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="B55" t="s">
-        <v>186</v>
-      </c>
-      <c r="C55" t="s">
-        <v>92</v>
-      </c>
-      <c r="D55" t="s">
-        <v>80</v>
-      </c>
-      <c r="E55" t="s">
-        <v>110</v>
-      </c>
-      <c r="F55" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="B56" t="s">
-        <v>187</v>
-      </c>
-      <c r="C56" t="s">
-        <v>92</v>
-      </c>
-      <c r="D56" t="s">
-        <v>80</v>
-      </c>
-      <c r="E56" t="s">
-        <v>112</v>
-      </c>
-      <c r="F56" t="s">
-        <v>58</v>
-      </c>
-    </row>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
   </sheetData>
   <sheetProtection sheet="0" objects="0" scenarios="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <mergeCells count="1">

</xml_diff>